<commit_message>
Add Apocalypse and Final Project datasets
</commit_message>
<xml_diff>
--- a/Datasets/Power BI - Final Project.xlsx
+++ b/Datasets/Power BI - Final Project.xlsx
@@ -5831,15 +5831,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB631"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="30" customWidth="1"/>
-    <col min="3" max="4" width="29" customWidth="1"/>
+    <col min="3" max="3" width="32.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>

</xml_diff>